<commit_message>
Gros commit concernant les issues #15 , #13 et #18.
Mise en place du champ référence client, completement optionnel, qui ne doit pas forcement figurer sur le fichier excel. Mais il doit cependant être présent dans Jira sous le nom précis :"Reference client".

La lecture des pages du fichier excel se fait maintenant par le nom ce qui supprime les problèmes de configuration.

Une story terminée ne sera plus update.

Les parametres de configuration qui permettent de mettre à jour la priorité des story et des subtasks fonctionne.
</commit_message>
<xml_diff>
--- a/JiraLoader/jiraLoader-core/src/test/resources/excelFilesValidationTests/Import_JIRA_OK.xlsx
+++ b/JiraLoader/jiraLoader-core/src/test/resources/excelFilesValidationTests/Import_JIRA_OK.xlsx
@@ -235,10 +235,10 @@
     <t>true</t>
   </si>
   <si>
-    <t>Référence Client</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M5T_G01R12C06_BCA_KPSA_1048_1 </t>
+    <t>M5T_G01R12C06_BCA_KPSA_1048_1</t>
+  </si>
+  <si>
+    <t>Référence client</t>
   </si>
 </sst>
 </file>
@@ -481,10 +481,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -789,7 +789,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -811,10 +811,10 @@
       <c r="C1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="F1" s="17"/>
+      <c r="F1" s="18"/>
       <c r="G1" s="13" t="s">
         <v>45</v>
       </c>
@@ -988,7 +988,7 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -996,7 +996,7 @@
     <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="25.7109375" customWidth="1"/>
+    <col min="5" max="5" width="38.42578125" customWidth="1"/>
     <col min="6" max="6" width="74.85546875" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="46.28515625" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="7" bestFit="1" customWidth="1" collapsed="1"/>
@@ -1018,7 +1018,7 @@
         <v>0</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F1" s="12" t="s">
         <v>2</v>
@@ -1047,7 +1047,7 @@
       <c r="D2" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="18"/>
+      <c r="E2" s="17"/>
       <c r="G2" s="10"/>
       <c r="H2" s="10"/>
       <c r="I2" s="10"/>
@@ -1085,7 +1085,7 @@
         <v>33</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>53</v>

</xml_diff>